<commit_message>
Solutions for the 1,2,5 and 6 problems
</commit_message>
<xml_diff>
--- a/1way Annova/onewayannova test.xlsx
+++ b/1way Annova/onewayannova test.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/kumarsg_adobe_com/Documents/Personal/BIA/data-science/1way Annova/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumarsg\OneDrive - Adobe Systems Incorporated\Personal\BIA\data-science\1way Annova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{BC01AB92-A5EB-4CE5-9845-72FF70B051A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3E8013DC-2A62-42A6-8616-CE8D192CF94D}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{BC01AB92-A5EB-4CE5-9845-72FF70B051A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4297BFD1-F4F6-495D-A320-0DA272EC5CD6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{232D4872-0F4F-4206-B4C4-C225C6E127B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{232D4872-0F4F-4206-B4C4-C225C6E127B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem" sheetId="1" r:id="rId1"/>
     <sheet name="data and soln" sheetId="2" r:id="rId2"/>
+    <sheet name="reliance discount" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Ex 7.1 from the Book Business Data Analytics</t>
   </si>
@@ -151,6 +152,27 @@
   </si>
   <si>
     <t>Anova: Single Factor - Generated using data analysis tool in excel</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>0% disc</t>
+  </si>
+  <si>
+    <t>10% disc</t>
+  </si>
+  <si>
+    <t>20% disc</t>
+  </si>
+  <si>
+    <t>Enzo</t>
+  </si>
+  <si>
+    <t>SUDZ</t>
+  </si>
+  <si>
+    <t>Anova: Single Factor</t>
   </si>
 </sst>
 </file>
@@ -278,7 +300,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -288,6 +310,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951C13E-BABF-4BC8-9F35-D269F5CC5AA6}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,4 +1314,311 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B9C293-9605-4FFA-B039-58B79F32E09D}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="H1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6">
+        <v>39</v>
+      </c>
+      <c r="D15" s="6">
+        <v>13</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6">
+        <v>33</v>
+      </c>
+      <c r="D16" s="6">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <v>36</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="6">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.62973760932944622</v>
+      </c>
+      <c r="G22" s="6">
+        <v>5.1432528497847176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="6">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6">
+        <v>6</v>
+      </c>
+      <c r="D23" s="6">
+        <v>6</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="7">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7">
+        <v>8</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>